<commit_message>
logged invalid dates issue while saving on sundays
</commit_message>
<xml_diff>
--- a/Timesheet improvements.xlsx
+++ b/Timesheet improvements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vasu\Timesheets\Timesheet application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6048D9-AB9A-430C-B82E-20A5845392D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15EC5B-38F7-4E3A-83EF-E108CC07592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Issues</t>
   </si>
@@ -40,6 +40,21 @@
   </si>
   <si>
     <t>Night shift employees timing issue</t>
+  </si>
+  <si>
+    <t>Day &amp; Night shift dropdown</t>
+  </si>
+  <si>
+    <t>Shared Services separation</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Phases</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
   </si>
 </sst>
 </file>
@@ -366,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -378,25 +393,50 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>